<commit_message>
FIX BUG IN INPUT
</commit_message>
<xml_diff>
--- a/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
+++ b/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B298266-5519-EF4A-A1BB-9B7F82E20678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EC69F8-C505-3140-9E35-66B9A6A7A28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="21" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Meanings" sheetId="1" r:id="rId1"/>
@@ -3267,7 +3267,9 @@
   </sheetPr>
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -17080,8 +17082,8 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="A48" sqref="A48"/>

</xml_diff>

<commit_message>
Fix bug for generate.py
</commit_message>
<xml_diff>
--- a/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
+++ b/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EC69F8-C505-3140-9E35-66B9A6A7A28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F32E686-5BF8-1945-8077-319E4A3A106F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Meanings" sheetId="1" r:id="rId1"/>
@@ -273,12 +273,6 @@
     <t>COMP 790-158 Special Topics: Special topics in Natural Language Processing</t>
   </si>
   <si>
-    <t>COMP 790-150   Special Topics: Efficient Deep Learning</t>
-  </si>
-  <si>
-    <t>COMP 790-189   Special Topics: Theoretical Foundations of Machine Learning</t>
-  </si>
-  <si>
     <t>COMP 89H - 063</t>
   </si>
   <si>
@@ -310,9 +304,6 @@
   </si>
   <si>
     <t>COMP 790-185 Special Topics: Research Topics in Computer Security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMP  790-188   Special Topics: Topics in Applied Cryptography        </t>
   </si>
   <si>
     <t>COMP 590-080   Special Topics: Video Compression and Streaming</t>
@@ -352,6 +343,15 @@
   </si>
   <si>
     <t>COMP 590-159 Special Topics: Interactive Computer Graphics using WebGL and HTML5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMP 790-188 Special Topics: Topics in Applied Cryptography        </t>
+  </si>
+  <si>
+    <t>COMP 790-189 Special Topics: Theoretical Foundations of Machine Learning</t>
+  </si>
+  <si>
+    <t>COMP 790-150 Special Topics: Efficient Deep Learning</t>
   </si>
 </sst>
 </file>
@@ -1401,11 +1401,11 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2063,7 +2063,9 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2579,7 +2581,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -3241,7 +3243,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -3267,7 +3269,7 @@
   </sheetPr>
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -3785,7 +3787,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -4078,7 +4080,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4842,7 +4844,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4856,7 +4858,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4969,7 +4971,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5117,7 +5119,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -10310,7 +10312,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10555,7 +10557,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11929,7 +11931,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13242,7 +13244,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13271,7 +13273,9 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -13787,7 +13791,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -15751,7 +15755,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -16070,7 +16074,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17718,7 +17722,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -19031,7 +19035,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -20344,7 +20348,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -22745,7 +22749,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -24589,7 +24593,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -25251,7 +25255,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -26564,7 +26568,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27226,7 +27230,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27787,7 +27791,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -29193,7 +29197,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -29858,7 +29862,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Fix the bug for Kandel
</commit_message>
<xml_diff>
--- a/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
+++ b/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F32E686-5BF8-1945-8077-319E4A3A106F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6388D5C6-0D01-E24E-9D75-7341A4A9E7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="10" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Meanings" sheetId="1" r:id="rId1"/>
@@ -300,9 +300,6 @@
     <t>I believe teaching 423 at scale will always win out over 523.</t>
   </si>
   <si>
-    <t>COMP 590-173   Special Topics: Information Visualization</t>
-  </si>
-  <si>
     <t>COMP 790-185 Special Topics: Research Topics in Computer Security</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>COMP 790-150 Special Topics: Efficient Deep Learning</t>
+  </si>
+  <si>
+    <t>COMP 590-173 Special Topics: Information Visualization</t>
   </si>
 </sst>
 </file>
@@ -1401,7 +1401,7 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -11415,7 +11415,9 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -11931,7 +11933,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13244,7 +13246,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13791,7 +13793,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -15755,7 +15757,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -16074,7 +16076,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17722,7 +17724,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -19035,7 +19037,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -20348,7 +20350,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -22749,7 +22751,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -24593,7 +24595,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -25255,7 +25257,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -26568,7 +26570,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27230,7 +27232,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27791,7 +27793,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -29197,7 +29199,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -29862,7 +29864,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Fix the input for Stotts
</commit_message>
<xml_diff>
--- a/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
+++ b/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6388D5C6-0D01-E24E-9D75-7341A4A9E7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6E5334-B921-E843-8357-AD86179215F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="10" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="28" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Meanings" sheetId="1" r:id="rId1"/>
@@ -324,9 +324,6 @@
     <t>COMP 664 Deep Learning</t>
   </si>
   <si>
-    <t>COMP 590-059   Special Topics: Special topics: Programming Methods, Models, Languages, and Analysis</t>
-  </si>
-  <si>
     <t>COMP 637 Formal Methods for Systems Security</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>COMP 590-173 Special Topics: Information Visualization</t>
+  </si>
+  <si>
+    <t>COMP 590-059 Special Topics: Special topics: Programming Methods, Models, Languages, and Analysis</t>
   </si>
 </sst>
 </file>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -11415,8 +11415,8 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11933,7 +11933,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13793,7 +13793,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -17724,7 +17724,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -25934,11 +25934,11 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -26570,7 +26570,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27232,7 +27232,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27793,7 +27793,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -29199,7 +29199,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -29864,7 +29864,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Fix input for Sengupta
</commit_message>
<xml_diff>
--- a/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
+++ b/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6E5334-B921-E843-8357-AD86179215F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279F752F-B9F8-844C-B943-5B616B71EC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="28" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="28" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Meanings" sheetId="1" r:id="rId1"/>
@@ -315,9 +315,6 @@
     <t>COMP 590&amp;790-187 Special Topics: Building the Infinite Brain</t>
   </si>
   <si>
-    <t>COMP 590-177   Special Topics: Introduction to Computer Vision</t>
-  </si>
-  <si>
     <t>COMP 651 Computational Geometry</t>
   </si>
   <si>
@@ -352,6 +349,9 @@
   </si>
   <si>
     <t>COMP 590-059 Special Topics: Special topics: Programming Methods, Models, Languages, and Analysis</t>
+  </si>
+  <si>
+    <t>COMP 590-177 Special Topics: Introduction to Computer Vision</t>
   </si>
 </sst>
 </file>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -11933,7 +11933,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13793,7 +13793,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -17724,7 +17724,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -22115,11 +22115,11 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -22751,7 +22751,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -24595,7 +24595,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -25257,7 +25257,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -25934,7 +25934,7 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -26570,7 +26570,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27232,7 +27232,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27793,7 +27793,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -29199,7 +29199,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -29864,7 +29864,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Fix the input for KMP and Chakravarthula
</commit_message>
<xml_diff>
--- a/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
+++ b/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279F752F-B9F8-844C-B943-5B616B71EC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76E7D71-8F19-704F-8751-413AE42090BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="28" activeTab="40" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Meanings" sheetId="1" r:id="rId1"/>
@@ -267,9 +267,6 @@
     <t>COMP 750 Algorithm Analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">COMP 590&amp;790-175   Special Topics: Visual Computing Systems        </t>
-  </si>
-  <si>
     <t>COMP 790-158 Special Topics: Special topics in Natural Language Processing</t>
   </si>
   <si>
@@ -301,9 +298,6 @@
   </si>
   <si>
     <t>COMP 790-185 Special Topics: Research Topics in Computer Security</t>
-  </si>
-  <si>
-    <t>COMP 590-080   Special Topics: Video Compression and Streaming</t>
   </si>
   <si>
     <t>I prefer to only teach this in the summer</t>
@@ -352,6 +346,12 @@
   </si>
   <si>
     <t>COMP 590-177 Special Topics: Introduction to Computer Vision</t>
+  </si>
+  <si>
+    <t>COMP 590-080 Special Topics: Video Compression and Streaming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMP 590&amp;790-175 Special Topics: Visual Computing Systems        </t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -3787,7 +3787,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -4080,7 +4080,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4844,7 +4844,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4858,7 +4858,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4971,7 +4971,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5119,7 +5119,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -10312,7 +10312,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10557,7 +10557,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11933,7 +11933,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13246,7 +13246,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13793,7 +13793,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -15125,7 +15125,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15757,7 +15757,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -16076,7 +16076,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17724,7 +17724,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -19037,7 +19037,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -20350,7 +20350,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -22115,7 +22115,7 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -22751,7 +22751,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -24595,7 +24595,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -25257,7 +25257,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -26570,7 +26570,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27232,7 +27232,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27793,7 +27793,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -29199,7 +29199,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -29864,7 +29864,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -31846,11 +31846,11 @@
   </sheetPr>
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -32482,7 +32482,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Now can fully generate all class no bugs
</commit_message>
<xml_diff>
--- a/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
+++ b/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76E7D71-8F19-704F-8751-413AE42090BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CDC998-E9C5-4740-A0A4-C2A817CC4DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Meanings" sheetId="1" r:id="rId1"/>
@@ -267,9 +267,6 @@
     <t>COMP 750 Algorithm Analysis</t>
   </si>
   <si>
-    <t>COMP 790-158 Special Topics: Special topics in Natural Language Processing</t>
-  </si>
-  <si>
     <t>COMP 89H - 063</t>
   </si>
   <si>
@@ -342,16 +339,19 @@
     <t>COMP 590-173 Special Topics: Information Visualization</t>
   </si>
   <si>
-    <t>COMP 590-059 Special Topics: Special topics: Programming Methods, Models, Languages, and Analysis</t>
-  </si>
-  <si>
     <t>COMP 590-177 Special Topics: Introduction to Computer Vision</t>
   </si>
   <si>
-    <t>COMP 590-080 Special Topics: Video Compression and Streaming</t>
+    <t xml:space="preserve">COMP 590&amp;790-175 Special Topics: Visual Computing Systems        </t>
   </si>
   <si>
-    <t xml:space="preserve">COMP 590&amp;790-175 Special Topics: Visual Computing Systems        </t>
+    <t>COMP 590-59 Special Topics: Special topics: Programming Methods, Models, Languages, and Analysis</t>
+  </si>
+  <si>
+    <t>COMP 590-80 Special Topics: Video Compression and Streaming</t>
+  </si>
+  <si>
+    <t>COMP 590&amp;790-158 Special Topics: Special topics in Natural Language Processing</t>
   </si>
 </sst>
 </file>
@@ -739,11 +739,11 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -3787,7 +3787,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -4080,7 +4080,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4844,7 +4844,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4858,7 +4858,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4971,7 +4971,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5119,7 +5119,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -10312,7 +10312,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10557,7 +10557,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11933,7 +11933,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13246,7 +13246,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -13793,7 +13793,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -16076,7 +16076,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -17724,7 +17724,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -19037,7 +19037,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -19718,7 +19718,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20350,7 +20350,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -22751,7 +22751,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -23312,7 +23312,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24595,7 +24595,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -25257,7 +25257,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -26570,7 +26570,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27232,7 +27232,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -27793,7 +27793,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -29199,7 +29199,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -29864,7 +29864,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>
@@ -31846,7 +31846,7 @@
   </sheetPr>
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -32482,7 +32482,7 @@
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B48" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Now schedule.py can work perfectly
</commit_message>
<xml_diff>
--- a/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
+++ b/data/Input/(For 523 team) Copy of Undergraduate Curriculum Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CDC998-E9C5-4740-A0A4-C2A817CC4DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DA51F1-0C5E-5742-9E44-A25D401334C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value Meanings" sheetId="1" r:id="rId1"/>
@@ -743,7 +743,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1290,10 +1290,10 @@
         <v>55</v>
       </c>
       <c r="B40" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C40" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7627,7 +7627,7 @@
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>